<commit_message>
Search all rule tree.
</commit_message>
<xml_diff>
--- a/tests/morpheme_merger/test_rules.xlsx
+++ b/tests/morpheme_merger/test_rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>pos0</t>
     <phoneticPr fontId="1"/>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>係助詞</t>
-  </si>
-  <si>
-    <t>副詞可能</t>
   </si>
   <si>
     <t>名詞</t>
@@ -142,13 +139,54 @@
   </si>
   <si>
     <t>助動詞</t>
+  </si>
+  <si>
+    <t>副詞可能</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rule3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>唖然と</t>
+    <rPh sb="0" eb="2">
+      <t>アゼント</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一般</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rule4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>申し訳ない</t>
+    <rPh sb="0" eb="1">
+      <t>モウシワケナイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>連体化|並立助詞</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>形容動詞語幹|一般|ナイ形容詞語幹</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,6 +220,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +246,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -254,12 +300,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -286,6 +335,7 @@
     <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -313,6 +363,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -587,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -637,21 +688,21 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -659,19 +710,63 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -683,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -735,7 +830,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -743,10 +838,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -754,10 +849,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>